<commit_message>
fix bootstrapping, add border and auto width when saving excel
</commit_message>
<xml_diff>
--- a/result/cleaned_bootstrapping.xlsx
+++ b/result/cleaned_bootstrapping.xlsx
@@ -67,7 +67,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -433,13 +433,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="11.6" customWidth="1" min="1" max="1"/>
+    <col width="24.8" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="15.2" customWidth="1" min="4" max="4"/>
+    <col width="10.4" customWidth="1" min="5" max="5"/>
+    <col width="21.2" customWidth="1" min="6" max="6"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
@@ -500,44 +508,44 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>D → PK</t>
+          <t>BKD → PK</t>
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>0.17</v>
+        <v>0.036</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>0.033</v>
+        <v>0.036</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>5174</v>
+        <v>0.993</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>0</v>
+        <v>0.161</v>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>Signifikan</t>
+          <t>Tidak signifikan</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>P → PK</t>
+          <t>D → PK</t>
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>0.08799999999999999</v>
+        <v>0.17</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>0.036</v>
+        <v>0.033</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>2461</v>
+        <v>5174</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>0.007</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
@@ -548,24 +556,96 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
+          <t>P → PK</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>2461</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>Signifikan</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>PD → PK</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>-0.044</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>0.041</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>1081</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>Tidak signifikan</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
           <t>WB → PK</t>
         </is>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B7" s="3" t="n">
         <v>0.137</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C7" s="3" t="n">
         <v>0.034</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D7" s="3" t="n">
         <v>3992</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E7" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="3" t="inlineStr">
+      <c r="F7" s="3" t="inlineStr">
         <is>
           <t>Signifikan</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>WBD → PK</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>0.263</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>0.397</v>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>Tidak signifikan</t>
         </is>
       </c>
     </row>

</xml_diff>